<commit_message>
Modified example in DANAC 2013 paper
</commit_message>
<xml_diff>
--- a/paper/DANAC2013/exp/TPC-H Query Runtimes.xlsx
+++ b/paper/DANAC2013/exp/TPC-H Query Runtimes.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23206"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15780" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Blatt1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -176,30 +176,8 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="33">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -228,39 +206,17 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="33">
+  <cellStyles count="11">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -590,10 +546,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:U24"/>
+  <dimension ref="A2:T24"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="O29" sqref="O29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R12" sqref="R12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -604,7 +560,7 @@
     <col min="17" max="17" width="4.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:21" ht="18">
+    <row r="2" spans="1:20" ht="18">
       <c r="A2" s="6" t="s">
         <v>4</v>
       </c>
@@ -630,7 +586,7 @@
       <c r="S2" s="5"/>
       <c r="T2" s="5"/>
     </row>
-    <row r="3" spans="1:21">
+    <row r="3" spans="1:20">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -680,7 +636,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:21">
+    <row r="4" spans="1:20">
       <c r="A4">
         <v>1</v>
       </c>
@@ -692,17 +648,13 @@
         <v>1</v>
       </c>
       <c r="L4" s="4">
-        <v>359.464</v>
+        <v>378.89699999999999</v>
       </c>
       <c r="M4" s="4">
         <v>1005.503</v>
       </c>
       <c r="N4" s="3">
         <v>55.502000000000002</v>
-      </c>
-      <c r="O4">
-        <f>L4/N4</f>
-        <v>6.4765954380022341</v>
       </c>
       <c r="Q4" s="3">
         <v>1</v>
@@ -711,7 +663,7 @@
       <c r="S4" s="3"/>
       <c r="T4" s="3"/>
     </row>
-    <row r="5" spans="1:21">
+    <row r="5" spans="1:20">
       <c r="A5">
         <v>2</v>
       </c>
@@ -723,17 +675,13 @@
         <v>2</v>
       </c>
       <c r="L5" s="4">
-        <v>315.21699999999998</v>
+        <v>363.97800000000001</v>
       </c>
       <c r="M5" s="4">
         <v>949.54300000000001</v>
       </c>
       <c r="N5" s="3">
         <v>46.258000000000003</v>
-      </c>
-      <c r="O5">
-        <f>L5/N5</f>
-        <v>6.8143240088200949</v>
       </c>
       <c r="Q5" s="3">
         <v>2</v>
@@ -742,7 +690,7 @@
       <c r="S5" s="3"/>
       <c r="T5" s="3"/>
     </row>
-    <row r="6" spans="1:21">
+    <row r="6" spans="1:20">
       <c r="A6">
         <v>3</v>
       </c>
@@ -755,7 +703,9 @@
       <c r="K6" s="3">
         <v>3</v>
       </c>
-      <c r="L6" s="3"/>
+      <c r="L6" s="3">
+        <v>374.30099999999999</v>
+      </c>
       <c r="M6" s="3"/>
       <c r="N6" s="3"/>
       <c r="Q6" s="3">
@@ -765,7 +715,7 @@
       <c r="S6" s="3"/>
       <c r="T6" s="3"/>
     </row>
-    <row r="7" spans="1:21">
+    <row r="7" spans="1:20">
       <c r="A7">
         <v>4</v>
       </c>
@@ -788,7 +738,7 @@
       <c r="S7" s="3"/>
       <c r="T7" s="3"/>
     </row>
-    <row r="8" spans="1:21">
+    <row r="8" spans="1:20">
       <c r="A8">
         <v>5</v>
       </c>
@@ -811,7 +761,7 @@
       <c r="S8" s="3"/>
       <c r="T8" s="3"/>
     </row>
-    <row r="10" spans="1:21" ht="18">
+    <row r="10" spans="1:20" ht="18">
       <c r="A10" s="5" t="s">
         <v>7</v>
       </c>
@@ -837,7 +787,7 @@
       <c r="S10" s="5"/>
       <c r="T10" s="5"/>
     </row>
-    <row r="11" spans="1:21">
+    <row r="11" spans="1:20">
       <c r="A11" s="2" t="s">
         <v>0</v>
       </c>
@@ -887,7 +837,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:21">
+    <row r="12" spans="1:20">
       <c r="A12" s="3">
         <v>1</v>
       </c>
@@ -898,15 +848,11 @@
         <v>1</v>
       </c>
       <c r="G12" s="3">
-        <v>499.327</v>
+        <v>553.23699999999997</v>
       </c>
       <c r="H12" s="3"/>
       <c r="I12" s="3">
         <v>85.346999999999994</v>
-      </c>
-      <c r="J12">
-        <f>G12/I12</f>
-        <v>5.8505512788967398</v>
       </c>
       <c r="K12" s="3">
         <v>1</v>
@@ -918,18 +864,14 @@
         <v>1</v>
       </c>
       <c r="R12" s="3">
-        <v>658.096</v>
+        <v>723.73299999999995</v>
       </c>
       <c r="S12" s="3"/>
       <c r="T12" s="3">
         <v>33.933</v>
       </c>
-      <c r="U12">
-        <f>R12/T12</f>
-        <v>19.393982259157752</v>
-      </c>
-    </row>
-    <row r="13" spans="1:21">
+    </row>
+    <row r="13" spans="1:20">
       <c r="A13" s="3">
         <v>2</v>
       </c>
@@ -940,15 +882,11 @@
         <v>2</v>
       </c>
       <c r="G13" s="3">
-        <v>488.77800000000002</v>
+        <v>533.92399999999998</v>
       </c>
       <c r="H13" s="3"/>
       <c r="I13" s="3">
         <v>70.522000000000006</v>
-      </c>
-      <c r="J13">
-        <f>G13/I13</f>
-        <v>6.9308584555174271</v>
       </c>
       <c r="K13" s="3">
         <v>2</v>
@@ -959,19 +897,13 @@
       <c r="Q13" s="3">
         <v>2</v>
       </c>
-      <c r="R13" s="3">
-        <v>658.096</v>
-      </c>
+      <c r="R13" s="3"/>
       <c r="S13" s="3"/>
       <c r="T13" s="3">
         <v>29.702999999999999</v>
       </c>
-      <c r="U13">
-        <f>R13/T13</f>
-        <v>22.155876510790158</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21">
+    </row>
+    <row r="14" spans="1:20">
       <c r="A14" s="3">
         <v>3</v>
       </c>
@@ -982,7 +914,7 @@
         <v>3</v>
       </c>
       <c r="G14" s="3">
-        <v>497.447</v>
+        <v>537.89300000000003</v>
       </c>
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
@@ -1001,7 +933,7 @@
         <v>28.449000000000002</v>
       </c>
     </row>
-    <row r="15" spans="1:21">
+    <row r="15" spans="1:20">
       <c r="A15" s="3">
         <v>4</v>
       </c>
@@ -1027,7 +959,7 @@
       <c r="S15" s="3"/>
       <c r="T15" s="3"/>
     </row>
-    <row r="16" spans="1:21">
+    <row r="16" spans="1:20">
       <c r="A16" s="3">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
Fixed distributed TPC-H Q20
</commit_message>
<xml_diff>
--- a/paper/DANAC2013/exp/TPC-H Query Runtimes.xlsx
+++ b/paper/DANAC2013/exp/TPC-H Query Runtimes.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="29">
   <si>
     <t>Run</t>
   </si>
@@ -64,14 +64,57 @@
   </si>
   <si>
     <t>Query BASKET</t>
+  </si>
+  <si>
+    <t>Query 10</t>
+  </si>
+  <si>
+    <t>Query 11</t>
+  </si>
+  <si>
+    <t>Query 12</t>
+  </si>
+  <si>
+    <t>Query 13</t>
+  </si>
+  <si>
+    <t>Query 14</t>
+  </si>
+  <si>
+    <t>Query 15</t>
+  </si>
+  <si>
+    <t>Query 16</t>
+  </si>
+  <si>
+    <t>Query 17</t>
+  </si>
+  <si>
+    <t>Query 18</t>
+  </si>
+  <si>
+    <t>Query 19</t>
+  </si>
+  <si>
+    <t>Query 20</t>
+  </si>
+  <si>
+    <t>Query 21</t>
+  </si>
+  <si>
+    <t>Query 22</t>
+  </si>
+  <si>
+    <t>n/a</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="#,##0.000"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -176,7 +219,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -188,8 +231,20 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -199,24 +254,41 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="23">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -546,10 +618,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:T24"/>
+  <dimension ref="A2:T64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R12" sqref="R12"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -561,30 +633,30 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:20" ht="18">
-      <c r="A2" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="F2" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="K2" s="5" t="s">
+      <c r="A2" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="F2" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="K2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-      <c r="Q2" s="5" t="s">
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
+      <c r="Q2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="R2" s="5"/>
-      <c r="S2" s="5"/>
-      <c r="T2" s="5"/>
+      <c r="R2" s="7"/>
+      <c r="S2" s="7"/>
+      <c r="T2" s="7"/>
     </row>
     <row r="3" spans="1:20">
       <c r="A3" s="1" t="s">
@@ -640,9 +712,20 @@
       <c r="A4">
         <v>1</v>
       </c>
-      <c r="D4" s="4"/>
+      <c r="B4">
+        <v>258.98700000000002</v>
+      </c>
+      <c r="D4" s="4">
+        <v>77.046000000000006</v>
+      </c>
       <c r="F4">
         <v>1</v>
+      </c>
+      <c r="G4" s="6">
+        <v>200.691</v>
+      </c>
+      <c r="I4">
+        <v>0.90300000000000002</v>
       </c>
       <c r="K4" s="3">
         <v>1</v>
@@ -654,7 +737,7 @@
         <v>1005.503</v>
       </c>
       <c r="N4" s="3">
-        <v>55.502000000000002</v>
+        <v>93.596000000000004</v>
       </c>
       <c r="Q4" s="3">
         <v>1</v>
@@ -667,9 +750,20 @@
       <c r="A5">
         <v>2</v>
       </c>
-      <c r="D5" s="4"/>
+      <c r="B5" s="5">
+        <v>258681</v>
+      </c>
+      <c r="D5" s="4">
+        <v>77.251999999999995</v>
+      </c>
       <c r="F5">
         <v>2</v>
+      </c>
+      <c r="G5">
+        <v>204.559</v>
+      </c>
+      <c r="I5">
+        <v>0.69099999999999995</v>
       </c>
       <c r="K5" s="3">
         <v>2</v>
@@ -681,7 +775,7 @@
         <v>949.54300000000001</v>
       </c>
       <c r="N5" s="3">
-        <v>46.258000000000003</v>
+        <v>83.215999999999994</v>
       </c>
       <c r="Q5" s="3">
         <v>2</v>
@@ -696,9 +790,14 @@
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
+      <c r="D6" s="4">
+        <v>77.153000000000006</v>
+      </c>
       <c r="F6">
         <v>3</v>
+      </c>
+      <c r="I6">
+        <v>0.54400000000000004</v>
       </c>
       <c r="K6" s="3">
         <v>3</v>
@@ -707,7 +806,9 @@
         <v>374.30099999999999</v>
       </c>
       <c r="M6" s="3"/>
-      <c r="N6" s="3"/>
+      <c r="N6" s="3">
+        <v>74.260000000000005</v>
+      </c>
       <c r="Q6" s="3">
         <v>3</v>
       </c>
@@ -762,30 +863,30 @@
       <c r="T8" s="3"/>
     </row>
     <row r="10" spans="1:20" ht="18">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="F10" s="5" t="s">
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="F10" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="K10" s="5" t="s">
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="K10" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="L10" s="5"/>
-      <c r="M10" s="5"/>
-      <c r="N10" s="5"/>
-      <c r="Q10" s="5" t="s">
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="7"/>
+      <c r="Q10" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="R10" s="5"/>
-      <c r="S10" s="5"/>
-      <c r="T10" s="5"/>
+      <c r="R10" s="7"/>
+      <c r="S10" s="7"/>
+      <c r="T10" s="7"/>
     </row>
     <row r="11" spans="1:20">
       <c r="A11" s="2" t="s">
@@ -841,9 +942,13 @@
       <c r="A12" s="3">
         <v>1</v>
       </c>
-      <c r="B12" s="3"/>
+      <c r="B12" s="3">
+        <v>146.809</v>
+      </c>
       <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
+      <c r="D12" s="3">
+        <v>22.145</v>
+      </c>
       <c r="F12" s="3">
         <v>1</v>
       </c>
@@ -852,14 +957,18 @@
       </c>
       <c r="H12" s="3"/>
       <c r="I12" s="3">
-        <v>85.346999999999994</v>
+        <v>53.372999999999998</v>
       </c>
       <c r="K12" s="3">
         <v>1</v>
       </c>
-      <c r="L12" s="3"/>
+      <c r="L12" s="3">
+        <v>140.44200000000001</v>
+      </c>
       <c r="M12" s="3"/>
-      <c r="N12" s="3"/>
+      <c r="N12" s="3">
+        <v>19.491</v>
+      </c>
       <c r="Q12" s="3">
         <v>1</v>
       </c>
@@ -875,9 +984,13 @@
       <c r="A13" s="3">
         <v>2</v>
       </c>
-      <c r="B13" s="3"/>
+      <c r="B13" s="3">
+        <v>148.41200000000001</v>
+      </c>
       <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
+      <c r="D13" s="3">
+        <v>21.69</v>
+      </c>
       <c r="F13" s="3">
         <v>2</v>
       </c>
@@ -886,18 +999,24 @@
       </c>
       <c r="H13" s="3"/>
       <c r="I13" s="3">
-        <v>70.522000000000006</v>
+        <v>53.558</v>
       </c>
       <c r="K13" s="3">
         <v>2</v>
       </c>
-      <c r="L13" s="3"/>
+      <c r="L13" s="3">
+        <v>131.38800000000001</v>
+      </c>
       <c r="M13" s="3"/>
-      <c r="N13" s="3"/>
+      <c r="N13" s="3">
+        <v>20.283999999999999</v>
+      </c>
       <c r="Q13" s="3">
         <v>2</v>
       </c>
-      <c r="R13" s="3"/>
+      <c r="R13" s="3">
+        <v>728.13099999999997</v>
+      </c>
       <c r="S13" s="3"/>
       <c r="T13" s="3">
         <v>29.702999999999999</v>
@@ -907,9 +1026,13 @@
       <c r="A14" s="3">
         <v>3</v>
       </c>
-      <c r="B14" s="3"/>
+      <c r="B14" s="3">
+        <v>147.36199999999999</v>
+      </c>
       <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
+      <c r="D14" s="3">
+        <v>21.613</v>
+      </c>
       <c r="F14" s="3">
         <v>3</v>
       </c>
@@ -917,13 +1040,17 @@
         <v>537.89300000000003</v>
       </c>
       <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
+      <c r="I14" s="3">
+        <v>53.284999999999997</v>
+      </c>
       <c r="K14" s="3">
         <v>3</v>
       </c>
       <c r="L14" s="3"/>
       <c r="M14" s="3"/>
-      <c r="N14" s="3"/>
+      <c r="N14" s="3">
+        <v>20.641999999999999</v>
+      </c>
       <c r="Q14" s="3">
         <v>3</v>
       </c>
@@ -986,24 +1113,24 @@
       <c r="T16" s="3"/>
     </row>
     <row r="18" spans="1:14" ht="18">
-      <c r="A18" s="5" t="s">
+      <c r="A18" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="F18" s="5" t="s">
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="F18" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-      <c r="K18" s="5" t="s">
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="7"/>
+      <c r="K18" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="L18" s="5"/>
-      <c r="M18" s="5"/>
-      <c r="N18" s="5"/>
+      <c r="L18" s="7"/>
+      <c r="M18" s="7"/>
+      <c r="N18" s="7"/>
     </row>
     <row r="19" spans="1:14">
       <c r="A19" s="2" t="s">
@@ -1047,41 +1174,65 @@
       <c r="A20" s="3">
         <v>1</v>
       </c>
-      <c r="B20" s="3"/>
+      <c r="B20" s="3">
+        <v>938.45899999999995</v>
+      </c>
       <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
+      <c r="D20" s="3">
+        <v>180.68799999999999</v>
+      </c>
       <c r="F20" s="3">
         <v>1</v>
       </c>
-      <c r="G20" s="3"/>
+      <c r="G20" s="3">
+        <v>567.40499999999997</v>
+      </c>
       <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
+      <c r="I20" s="3">
+        <v>242.279</v>
+      </c>
       <c r="K20" s="3">
         <v>1</v>
       </c>
-      <c r="L20" s="3"/>
+      <c r="L20" s="3">
+        <v>1352.076</v>
+      </c>
       <c r="M20" s="3"/>
-      <c r="N20" s="3"/>
+      <c r="N20" s="3">
+        <v>438.89100000000002</v>
+      </c>
     </row>
     <row r="21" spans="1:14">
       <c r="A21" s="3">
         <v>2</v>
       </c>
-      <c r="B21" s="3"/>
+      <c r="B21" s="3">
+        <v>957.52300000000002</v>
+      </c>
       <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
+      <c r="D21" s="3">
+        <v>166.68799999999999</v>
+      </c>
       <c r="F21" s="3">
         <v>2</v>
       </c>
-      <c r="G21" s="3"/>
+      <c r="G21" s="3">
+        <v>579.61599999999999</v>
+      </c>
       <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
+      <c r="I21" s="3">
+        <v>194.21299999999999</v>
+      </c>
       <c r="K21" s="3">
         <v>2</v>
       </c>
-      <c r="L21" s="3"/>
+      <c r="L21" s="3">
+        <v>1348.6849999999999</v>
+      </c>
       <c r="M21" s="3"/>
-      <c r="N21" s="3"/>
+      <c r="N21" s="3">
+        <v>441.05700000000002</v>
+      </c>
     </row>
     <row r="22" spans="1:14">
       <c r="A22" s="3">
@@ -1089,19 +1240,27 @@
       </c>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
+      <c r="D22" s="3">
+        <v>151.756</v>
+      </c>
       <c r="F22" s="3">
         <v>3</v>
       </c>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
+      <c r="I22" s="3">
+        <v>169.61199999999999</v>
+      </c>
       <c r="K22" s="3">
         <v>3</v>
       </c>
-      <c r="L22" s="3"/>
+      <c r="L22" s="3">
+        <v>1347.0840000000001</v>
+      </c>
       <c r="M22" s="3"/>
-      <c r="N22" s="3"/>
+      <c r="N22" s="3">
+        <v>442.685</v>
+      </c>
     </row>
     <row r="23" spans="1:14">
       <c r="A23" s="3">
@@ -1115,7 +1274,9 @@
       </c>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
-      <c r="I23" s="3"/>
+      <c r="I23" s="3">
+        <v>142.756</v>
+      </c>
       <c r="K23" s="3">
         <v>4</v>
       </c>
@@ -1143,8 +1304,794 @@
       <c r="M24" s="3"/>
       <c r="N24" s="3"/>
     </row>
+    <row r="26" spans="1:14" ht="18">
+      <c r="A26" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="F26" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G26" s="7"/>
+      <c r="H26" s="7"/>
+      <c r="I26" s="7"/>
+      <c r="K26" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="L26" s="7"/>
+      <c r="M26" s="7"/>
+      <c r="N26" s="7"/>
+    </row>
+    <row r="27" spans="1:14">
+      <c r="A27" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="K27" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L27" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M27" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="N27" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14">
+      <c r="A28" s="3">
+        <v>1</v>
+      </c>
+      <c r="B28" s="3">
+        <v>362.33300000000003</v>
+      </c>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3">
+        <v>92.542000000000002</v>
+      </c>
+      <c r="F28" s="3">
+        <v>1</v>
+      </c>
+      <c r="G28" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3">
+        <v>19.395</v>
+      </c>
+      <c r="K28" s="3">
+        <v>1</v>
+      </c>
+      <c r="L28" s="3">
+        <v>246.583</v>
+      </c>
+      <c r="M28" s="3"/>
+      <c r="N28" s="3">
+        <v>56.103000000000002</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14">
+      <c r="A29" s="3">
+        <v>2</v>
+      </c>
+      <c r="B29" s="3">
+        <v>358.43700000000001</v>
+      </c>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3">
+        <v>35.881999999999998</v>
+      </c>
+      <c r="F29" s="3">
+        <v>2</v>
+      </c>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3">
+        <v>14.628</v>
+      </c>
+      <c r="K29" s="3">
+        <v>2</v>
+      </c>
+      <c r="L29" s="3">
+        <v>239.68100000000001</v>
+      </c>
+      <c r="M29" s="3"/>
+      <c r="N29" s="3">
+        <v>57.143000000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14">
+      <c r="A30" s="3">
+        <v>3</v>
+      </c>
+      <c r="B30" s="3">
+        <v>369.64100000000002</v>
+      </c>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3">
+        <v>35.917000000000002</v>
+      </c>
+      <c r="F30" s="3">
+        <v>3</v>
+      </c>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+      <c r="I30" s="3">
+        <v>13.516</v>
+      </c>
+      <c r="K30" s="3">
+        <v>3</v>
+      </c>
+      <c r="L30" s="3">
+        <v>237.49799999999999</v>
+      </c>
+      <c r="M30" s="3"/>
+      <c r="N30" s="3">
+        <v>56.683</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14">
+      <c r="A31" s="3">
+        <v>4</v>
+      </c>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="F31" s="3">
+        <v>4</v>
+      </c>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="3"/>
+      <c r="K31" s="3">
+        <v>4</v>
+      </c>
+      <c r="L31" s="3"/>
+      <c r="M31" s="3"/>
+      <c r="N31" s="3"/>
+    </row>
+    <row r="32" spans="1:14">
+      <c r="A32" s="3">
+        <v>5</v>
+      </c>
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="F32" s="3">
+        <v>5</v>
+      </c>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
+      <c r="I32" s="3"/>
+      <c r="K32" s="3">
+        <v>5</v>
+      </c>
+      <c r="L32" s="3"/>
+      <c r="M32" s="3"/>
+      <c r="N32" s="3"/>
+    </row>
+    <row r="34" spans="1:14" ht="18">
+      <c r="A34" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B34" s="7"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="7"/>
+      <c r="F34" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G34" s="7"/>
+      <c r="H34" s="7"/>
+      <c r="I34" s="7"/>
+      <c r="K34" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="L34" s="7"/>
+      <c r="M34" s="7"/>
+      <c r="N34" s="7"/>
+    </row>
+    <row r="35" spans="1:14">
+      <c r="A35" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I35" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="K35" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L35" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M35" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="N35" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14">
+      <c r="A36" s="3">
+        <v>1</v>
+      </c>
+      <c r="B36" s="3">
+        <v>214.54599999999999</v>
+      </c>
+      <c r="C36" s="3"/>
+      <c r="D36" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="F36" s="3">
+        <v>1</v>
+      </c>
+      <c r="G36" s="3">
+        <v>166.34100000000001</v>
+      </c>
+      <c r="H36" s="3"/>
+      <c r="I36" s="3">
+        <v>32.713999999999999</v>
+      </c>
+      <c r="K36" s="3">
+        <v>1</v>
+      </c>
+      <c r="L36" s="3">
+        <v>70.233000000000004</v>
+      </c>
+      <c r="M36" s="3"/>
+      <c r="N36" s="9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14">
+      <c r="A37" s="3">
+        <v>2</v>
+      </c>
+      <c r="B37" s="3">
+        <v>213.55699999999999</v>
+      </c>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
+      <c r="F37" s="3">
+        <v>2</v>
+      </c>
+      <c r="G37" s="3">
+        <v>163.077</v>
+      </c>
+      <c r="H37" s="3"/>
+      <c r="I37" s="3">
+        <v>20.044</v>
+      </c>
+      <c r="K37" s="3">
+        <v>2</v>
+      </c>
+      <c r="L37" s="3">
+        <v>71.257000000000005</v>
+      </c>
+      <c r="M37" s="3"/>
+      <c r="N37" s="3"/>
+    </row>
+    <row r="38" spans="1:14">
+      <c r="A38" s="3">
+        <v>3</v>
+      </c>
+      <c r="B38" s="3">
+        <v>207.31899999999999</v>
+      </c>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
+      <c r="F38" s="3">
+        <v>3</v>
+      </c>
+      <c r="G38" s="3">
+        <v>165.346</v>
+      </c>
+      <c r="H38" s="3"/>
+      <c r="I38" s="3">
+        <v>21.190999999999999</v>
+      </c>
+      <c r="K38" s="3">
+        <v>3</v>
+      </c>
+      <c r="L38" s="3">
+        <v>73.286000000000001</v>
+      </c>
+      <c r="M38" s="3"/>
+      <c r="N38" s="3"/>
+    </row>
+    <row r="39" spans="1:14">
+      <c r="A39" s="3">
+        <v>4</v>
+      </c>
+      <c r="B39" s="3"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+      <c r="F39" s="3">
+        <v>4</v>
+      </c>
+      <c r="G39" s="3"/>
+      <c r="H39" s="3"/>
+      <c r="I39" s="3"/>
+      <c r="K39" s="3">
+        <v>4</v>
+      </c>
+      <c r="L39" s="3"/>
+      <c r="M39" s="3"/>
+      <c r="N39" s="3"/>
+    </row>
+    <row r="40" spans="1:14">
+      <c r="A40" s="3">
+        <v>5</v>
+      </c>
+      <c r="B40" s="3"/>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3"/>
+      <c r="F40" s="3">
+        <v>5</v>
+      </c>
+      <c r="G40" s="3"/>
+      <c r="H40" s="3"/>
+      <c r="I40" s="3"/>
+      <c r="K40" s="3">
+        <v>5</v>
+      </c>
+      <c r="L40" s="3"/>
+      <c r="M40" s="3"/>
+      <c r="N40" s="3"/>
+    </row>
+    <row r="42" spans="1:14" ht="18">
+      <c r="A42" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B42" s="7"/>
+      <c r="C42" s="7"/>
+      <c r="D42" s="7"/>
+      <c r="F42" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G42" s="7"/>
+      <c r="H42" s="7"/>
+      <c r="I42" s="7"/>
+      <c r="K42" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="L42" s="7"/>
+      <c r="M42" s="7"/>
+      <c r="N42" s="7"/>
+    </row>
+    <row r="43" spans="1:14">
+      <c r="A43" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H43" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I43" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="K43" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L43" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M43" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="N43" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14">
+      <c r="A44" s="3">
+        <v>1</v>
+      </c>
+      <c r="B44" s="3">
+        <v>84.858000000000004</v>
+      </c>
+      <c r="C44" s="3"/>
+      <c r="D44" s="3">
+        <v>2.76</v>
+      </c>
+      <c r="F44" s="3">
+        <v>1</v>
+      </c>
+      <c r="G44" s="3"/>
+      <c r="H44" s="3"/>
+      <c r="I44" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="K44" s="3">
+        <v>1</v>
+      </c>
+      <c r="L44" s="3"/>
+      <c r="M44" s="3"/>
+      <c r="N44" s="3">
+        <v>26.486999999999998</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14">
+      <c r="A45" s="3">
+        <v>2</v>
+      </c>
+      <c r="B45" s="3"/>
+      <c r="C45" s="3"/>
+      <c r="D45" s="3">
+        <v>1.085</v>
+      </c>
+      <c r="F45" s="3">
+        <v>2</v>
+      </c>
+      <c r="G45" s="3"/>
+      <c r="H45" s="3"/>
+      <c r="I45" s="3"/>
+      <c r="K45" s="3">
+        <v>2</v>
+      </c>
+      <c r="L45" s="3"/>
+      <c r="M45" s="3"/>
+      <c r="N45" s="3">
+        <v>25.555</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14">
+      <c r="A46" s="3">
+        <v>3</v>
+      </c>
+      <c r="B46" s="3"/>
+      <c r="C46" s="3"/>
+      <c r="D46" s="3">
+        <v>1.083</v>
+      </c>
+      <c r="F46" s="3">
+        <v>3</v>
+      </c>
+      <c r="G46" s="3"/>
+      <c r="H46" s="3"/>
+      <c r="I46" s="3"/>
+      <c r="K46" s="3">
+        <v>3</v>
+      </c>
+      <c r="L46" s="3"/>
+      <c r="M46" s="3"/>
+      <c r="N46" s="3">
+        <v>24.349</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14">
+      <c r="A47" s="3">
+        <v>4</v>
+      </c>
+      <c r="B47" s="3"/>
+      <c r="C47" s="3"/>
+      <c r="D47" s="3"/>
+      <c r="F47" s="3">
+        <v>4</v>
+      </c>
+      <c r="G47" s="3"/>
+      <c r="H47" s="3"/>
+      <c r="I47" s="3"/>
+      <c r="K47" s="3">
+        <v>4</v>
+      </c>
+      <c r="L47" s="3"/>
+      <c r="M47" s="3"/>
+      <c r="N47" s="3"/>
+    </row>
+    <row r="48" spans="1:14">
+      <c r="A48" s="3">
+        <v>5</v>
+      </c>
+      <c r="B48" s="3"/>
+      <c r="C48" s="3"/>
+      <c r="D48" s="3"/>
+      <c r="F48" s="3">
+        <v>5</v>
+      </c>
+      <c r="G48" s="3"/>
+      <c r="H48" s="3"/>
+      <c r="I48" s="3"/>
+      <c r="K48" s="3">
+        <v>5</v>
+      </c>
+      <c r="L48" s="3"/>
+      <c r="M48" s="3"/>
+      <c r="N48" s="3"/>
+    </row>
+    <row r="50" spans="1:14" ht="18">
+      <c r="A50" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B50" s="7"/>
+      <c r="C50" s="7"/>
+      <c r="D50" s="7"/>
+      <c r="F50" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G50" s="7"/>
+      <c r="H50" s="7"/>
+      <c r="I50" s="7"/>
+      <c r="K50" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="L50" s="7"/>
+      <c r="M50" s="7"/>
+      <c r="N50" s="7"/>
+    </row>
+    <row r="51" spans="1:14">
+      <c r="A51" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G51" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H51" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I51" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="K51" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L51" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M51" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="N51" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14">
+      <c r="A52" s="3">
+        <v>1</v>
+      </c>
+      <c r="B52" s="3"/>
+      <c r="C52" s="3"/>
+      <c r="D52" s="3">
+        <v>31.056000000000001</v>
+      </c>
+      <c r="F52" s="3">
+        <v>1</v>
+      </c>
+      <c r="G52" s="3"/>
+      <c r="H52" s="3"/>
+      <c r="I52" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="K52" s="3">
+        <v>1</v>
+      </c>
+      <c r="L52" s="3"/>
+      <c r="M52" s="3"/>
+      <c r="N52" s="3">
+        <v>127.312</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14">
+      <c r="A53" s="3">
+        <v>2</v>
+      </c>
+      <c r="B53" s="3"/>
+      <c r="C53" s="3"/>
+      <c r="D53" s="3">
+        <v>31.265999999999998</v>
+      </c>
+      <c r="F53" s="3">
+        <v>2</v>
+      </c>
+      <c r="G53" s="3"/>
+      <c r="H53" s="3"/>
+      <c r="I53" s="3"/>
+      <c r="K53" s="3">
+        <v>2</v>
+      </c>
+      <c r="L53" s="3"/>
+      <c r="M53" s="3"/>
+      <c r="N53" s="3">
+        <v>119.833</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14">
+      <c r="A54" s="3">
+        <v>3</v>
+      </c>
+      <c r="B54" s="3"/>
+      <c r="C54" s="3"/>
+      <c r="D54" s="3">
+        <v>31.305</v>
+      </c>
+      <c r="F54" s="3">
+        <v>3</v>
+      </c>
+      <c r="G54" s="3"/>
+      <c r="H54" s="3"/>
+      <c r="I54" s="3"/>
+      <c r="K54" s="3">
+        <v>3</v>
+      </c>
+      <c r="L54" s="3"/>
+      <c r="M54" s="3"/>
+      <c r="N54" s="3">
+        <v>119.619</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14">
+      <c r="A55" s="3">
+        <v>4</v>
+      </c>
+      <c r="B55" s="3"/>
+      <c r="C55" s="3"/>
+      <c r="D55" s="3"/>
+      <c r="F55" s="3">
+        <v>4</v>
+      </c>
+      <c r="G55" s="3"/>
+      <c r="H55" s="3"/>
+      <c r="I55" s="3"/>
+      <c r="K55" s="3">
+        <v>4</v>
+      </c>
+      <c r="L55" s="3"/>
+      <c r="M55" s="3"/>
+      <c r="N55" s="3"/>
+    </row>
+    <row r="56" spans="1:14">
+      <c r="A56" s="3">
+        <v>5</v>
+      </c>
+      <c r="B56" s="3"/>
+      <c r="C56" s="3"/>
+      <c r="D56" s="3"/>
+      <c r="F56" s="3">
+        <v>5</v>
+      </c>
+      <c r="G56" s="3"/>
+      <c r="H56" s="3"/>
+      <c r="I56" s="3"/>
+      <c r="K56" s="3">
+        <v>5</v>
+      </c>
+      <c r="L56" s="3"/>
+      <c r="M56" s="3"/>
+      <c r="N56" s="3"/>
+    </row>
+    <row r="58" spans="1:14" ht="18">
+      <c r="A58" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B58" s="7"/>
+      <c r="C58" s="7"/>
+      <c r="D58" s="7"/>
+    </row>
+    <row r="59" spans="1:14">
+      <c r="A59" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14">
+      <c r="A60" s="3">
+        <v>1</v>
+      </c>
+      <c r="B60" s="3"/>
+      <c r="C60" s="3"/>
+      <c r="D60" s="9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14">
+      <c r="A61" s="3">
+        <v>2</v>
+      </c>
+      <c r="B61" s="3"/>
+      <c r="C61" s="3"/>
+      <c r="D61" s="3"/>
+    </row>
+    <row r="62" spans="1:14">
+      <c r="A62" s="3">
+        <v>3</v>
+      </c>
+      <c r="B62" s="3"/>
+      <c r="C62" s="3"/>
+      <c r="D62" s="3"/>
+    </row>
+    <row r="63" spans="1:14">
+      <c r="A63" s="3">
+        <v>4</v>
+      </c>
+      <c r="B63" s="3"/>
+      <c r="C63" s="3"/>
+      <c r="D63" s="3"/>
+    </row>
+    <row r="64" spans="1:14">
+      <c r="A64" s="3">
+        <v>5</v>
+      </c>
+      <c r="B64" s="3"/>
+      <c r="C64" s="3"/>
+      <c r="D64" s="3"/>
+    </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="24">
     <mergeCell ref="A18:D18"/>
     <mergeCell ref="F18:I18"/>
     <mergeCell ref="K18:N18"/>
@@ -1156,6 +2103,19 @@
     <mergeCell ref="F10:I10"/>
     <mergeCell ref="K10:N10"/>
     <mergeCell ref="Q10:T10"/>
+    <mergeCell ref="A26:D26"/>
+    <mergeCell ref="F26:I26"/>
+    <mergeCell ref="K26:N26"/>
+    <mergeCell ref="A34:D34"/>
+    <mergeCell ref="F34:I34"/>
+    <mergeCell ref="K34:N34"/>
+    <mergeCell ref="A58:D58"/>
+    <mergeCell ref="A42:D42"/>
+    <mergeCell ref="F42:I42"/>
+    <mergeCell ref="K42:N42"/>
+    <mergeCell ref="A50:D50"/>
+    <mergeCell ref="F50:I50"/>
+    <mergeCell ref="K50:N50"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>